<commit_message>
fixes: Adding New Stocks
</commit_message>
<xml_diff>
--- a/Record-Data.xlsx
+++ b/Record-Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="197">
   <si>
     <t>Daily as on Apr 1, 16:00</t>
   </si>
@@ -56,6 +56,555 @@
   </si>
   <si>
     <t>Bajaj Auto</t>
+  </si>
+  <si>
+    <t>IDFC First Bank</t>
+  </si>
+  <si>
+    <t>National Peroxide</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Philips Carbon</t>
+  </si>
+  <si>
+    <t>HEG</t>
+  </si>
+  <si>
+    <t>Bhartiya Airtel</t>
+  </si>
+  <si>
+    <t>Coal India</t>
+  </si>
+  <si>
+    <t>Wipro</t>
+  </si>
+  <si>
+    <t>I Bull Housing Finance</t>
+  </si>
+  <si>
+    <t>Idea</t>
+  </si>
+  <si>
+    <t>Indus Ind Bank</t>
+  </si>
+  <si>
+    <t>IOC</t>
+  </si>
+  <si>
+    <t>IRCTC</t>
+  </si>
+  <si>
+    <t>ITC</t>
+  </si>
+  <si>
+    <t>L&amp;T</t>
+  </si>
+  <si>
+    <t>M&amp;M Finance</t>
+  </si>
+  <si>
+    <t>Manapuram</t>
+  </si>
+  <si>
+    <t>Muthood Finance</t>
+  </si>
+  <si>
+    <t>PFC</t>
+  </si>
+  <si>
+    <t>SBI Life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI  </t>
+  </si>
+  <si>
+    <t>Tata Powers</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>Tata Chemicals</t>
+  </si>
+  <si>
+    <t>Hindal Co</t>
+  </si>
+  <si>
+    <t>Asian Paints</t>
+  </si>
+  <si>
+    <t>Adani Port</t>
+  </si>
+  <si>
+    <t>Sunpharma</t>
+  </si>
+  <si>
+    <t>Tata Steels</t>
+  </si>
+  <si>
+    <t>Deepak Nitrite</t>
+  </si>
+  <si>
+    <t>45.45</t>
+  </si>
+  <si>
+    <t>50.20</t>
+  </si>
+  <si>
+    <t>47.16</t>
+  </si>
+  <si>
+    <t>54.05</t>
+  </si>
+  <si>
+    <t>45.62</t>
+  </si>
+  <si>
+    <t>48.23</t>
+  </si>
+  <si>
+    <t>51.49</t>
+  </si>
+  <si>
+    <t>41.03</t>
+  </si>
+  <si>
+    <t>49.99</t>
+  </si>
+  <si>
+    <t>43.07</t>
+  </si>
+  <si>
+    <t>- -</t>
+  </si>
+  <si>
+    <t>50.76</t>
+  </si>
+  <si>
+    <t>52.29</t>
+  </si>
+  <si>
+    <t>59.05</t>
+  </si>
+  <si>
+    <t>41.86</t>
+  </si>
+  <si>
+    <t>39.57</t>
+  </si>
+  <si>
+    <t>48.86</t>
+  </si>
+  <si>
+    <t>42.67</t>
+  </si>
+  <si>
+    <t>47.21</t>
+  </si>
+  <si>
+    <t>48.65</t>
+  </si>
+  <si>
+    <t>41.16</t>
+  </si>
+  <si>
+    <t>45.84</t>
+  </si>
+  <si>
+    <t>57.52</t>
+  </si>
+  <si>
+    <t>50.63</t>
+  </si>
+  <si>
+    <t>50.27</t>
+  </si>
+  <si>
+    <t>45.61</t>
+  </si>
+  <si>
+    <t>43.41</t>
+  </si>
+  <si>
+    <t>37.58</t>
+  </si>
+  <si>
+    <t>47.48</t>
+  </si>
+  <si>
+    <t>49.80</t>
+  </si>
+  <si>
+    <t>56.54</t>
+  </si>
+  <si>
+    <t>58.02</t>
+  </si>
+  <si>
+    <t>64.37</t>
+  </si>
+  <si>
+    <t>53.14</t>
+  </si>
+  <si>
+    <t>59.65</t>
+  </si>
+  <si>
+    <t>60.25</t>
+  </si>
+  <si>
+    <t>55.37</t>
+  </si>
+  <si>
+    <t>71.78</t>
+  </si>
+  <si>
+    <t>67.78</t>
+  </si>
+  <si>
+    <t>50.84</t>
+  </si>
+  <si>
+    <t>68.29</t>
+  </si>
+  <si>
+    <t>59.15</t>
+  </si>
+  <si>
+    <t>61.93</t>
+  </si>
+  <si>
+    <t>58.41</t>
+  </si>
+  <si>
+    <t>56.84</t>
+  </si>
+  <si>
+    <t>55.32</t>
+  </si>
+  <si>
+    <t>46.38</t>
+  </si>
+  <si>
+    <t>57.04</t>
+  </si>
+  <si>
+    <t>64.20</t>
+  </si>
+  <si>
+    <t>57.24</t>
+  </si>
+  <si>
+    <t>61.90</t>
+  </si>
+  <si>
+    <t>70.13</t>
+  </si>
+  <si>
+    <t>48.42</t>
+  </si>
+  <si>
+    <t>47.30</t>
+  </si>
+  <si>
+    <t>60.51</t>
+  </si>
+  <si>
+    <t>49.42</t>
+  </si>
+  <si>
+    <t>48.51</t>
+  </si>
+  <si>
+    <t>58.94</t>
+  </si>
+  <si>
+    <t>49.86</t>
+  </si>
+  <si>
+    <t>59.50</t>
+  </si>
+  <si>
+    <t>55.79</t>
+  </si>
+  <si>
+    <t>62.99</t>
+  </si>
+  <si>
+    <t>61.15</t>
+  </si>
+  <si>
+    <t>46.27</t>
+  </si>
+  <si>
+    <t>51.38</t>
+  </si>
+  <si>
+    <t>50.35</t>
+  </si>
+  <si>
+    <t>52.75</t>
+  </si>
+  <si>
+    <t>67.21</t>
+  </si>
+  <si>
+    <t>70.90</t>
+  </si>
+  <si>
+    <t>64.01</t>
+  </si>
+  <si>
+    <t>78.21</t>
+  </si>
+  <si>
+    <t>57.16</t>
+  </si>
+  <si>
+    <t>60.22</t>
+  </si>
+  <si>
+    <t>77.12</t>
+  </si>
+  <si>
+    <t>58.23</t>
+  </si>
+  <si>
+    <t>78.07</t>
+  </si>
+  <si>
+    <t>82.81</t>
+  </si>
+  <si>
+    <t>61.83</t>
+  </si>
+  <si>
+    <t>64.87</t>
+  </si>
+  <si>
+    <t>65.02</t>
+  </si>
+  <si>
+    <t>63.58</t>
+  </si>
+  <si>
+    <t>64.90</t>
+  </si>
+  <si>
+    <t>64.17</t>
+  </si>
+  <si>
+    <t>60.82</t>
+  </si>
+  <si>
+    <t>51.47</t>
+  </si>
+  <si>
+    <t>61.89</t>
+  </si>
+  <si>
+    <t>62.09</t>
+  </si>
+  <si>
+    <t>50.58</t>
+  </si>
+  <si>
+    <t>64.61</t>
+  </si>
+  <si>
+    <t>57.07</t>
+  </si>
+  <si>
+    <t>57.57</t>
+  </si>
+  <si>
+    <t>38.95</t>
+  </si>
+  <si>
+    <t>75.00</t>
+  </si>
+  <si>
+    <t>40.10</t>
+  </si>
+  <si>
+    <t>41.98</t>
+  </si>
+  <si>
+    <t>49.63</t>
+  </si>
+  <si>
+    <t>42.01</t>
+  </si>
+  <si>
+    <t>66.70</t>
+  </si>
+  <si>
+    <t>50.10</t>
+  </si>
+  <si>
+    <t>60.98</t>
+  </si>
+  <si>
+    <t>54.38</t>
+  </si>
+  <si>
+    <t>53.05</t>
+  </si>
+  <si>
+    <t>62.44</t>
+  </si>
+  <si>
+    <t>54.19</t>
+  </si>
+  <si>
+    <t>55.61</t>
+  </si>
+  <si>
+    <t>62.51</t>
+  </si>
+  <si>
+    <t>71.82</t>
+  </si>
+  <si>
+    <t>71.58</t>
+  </si>
+  <si>
+    <t>66.12</t>
+  </si>
+  <si>
+    <t>46.15</t>
+  </si>
+  <si>
+    <t>68.20</t>
+  </si>
+  <si>
+    <t>78.35</t>
+  </si>
+  <si>
+    <t>61.76</t>
+  </si>
+  <si>
+    <t>72.71</t>
+  </si>
+  <si>
+    <t>89.49</t>
+  </si>
+  <si>
+    <t>2021.85</t>
+  </si>
+  <si>
+    <t>307.75</t>
+  </si>
+  <si>
+    <t>5272.15</t>
+  </si>
+  <si>
+    <t>9789.50</t>
+  </si>
+  <si>
+    <t>1486.75</t>
+  </si>
+  <si>
+    <t>691.00</t>
+  </si>
+  <si>
+    <t>2963.35</t>
+  </si>
+  <si>
+    <t>6923.90</t>
+  </si>
+  <si>
+    <t>3743.05</t>
+  </si>
+  <si>
+    <t>57.05</t>
+  </si>
+  <si>
+    <t>299.95</t>
+  </si>
+  <si>
+    <t>198.70</t>
+  </si>
+  <si>
+    <t>1580.90</t>
+  </si>
+  <si>
+    <t>520.80</t>
+  </si>
+  <si>
+    <t>132.15</t>
+  </si>
+  <si>
+    <t>416.40</t>
+  </si>
+  <si>
+    <t>204.65</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>993.30</t>
+  </si>
+  <si>
+    <t>93.15</t>
+  </si>
+  <si>
+    <t>1751.75</t>
+  </si>
+  <si>
+    <t>220.05</t>
+  </si>
+  <si>
+    <t>1444.60</t>
+  </si>
+  <si>
+    <t>204.30</t>
+  </si>
+  <si>
+    <t>157.30</t>
+  </si>
+  <si>
+    <t>1214.35</t>
+  </si>
+  <si>
+    <t>114.40</t>
+  </si>
+  <si>
+    <t>883.45</t>
+  </si>
+  <si>
+    <t>370.65</t>
+  </si>
+  <si>
+    <t>105.05</t>
+  </si>
+  <si>
+    <t>3165.00</t>
+  </si>
+  <si>
+    <t>779.10</t>
+  </si>
+  <si>
+    <t>8.45</t>
+  </si>
+  <si>
+    <t>2551.75</t>
+  </si>
+  <si>
+    <t>736.25</t>
+  </si>
+  <si>
+    <t>610.75</t>
+  </si>
+  <si>
+    <t>863.05</t>
+  </si>
+  <si>
+    <t>1646.75</t>
   </si>
 </sst>
 </file>
@@ -413,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,153 +989,660 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>45.45</v>
-      </c>
-      <c r="C2">
-        <v>50.84</v>
-      </c>
-      <c r="D2">
-        <v>61.83</v>
-      </c>
-      <c r="E2">
-        <v>2021.85</v>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>50.2</v>
-      </c>
-      <c r="C3">
-        <v>68.29000000000001</v>
-      </c>
-      <c r="D3">
-        <v>64.87</v>
-      </c>
-      <c r="E3">
-        <v>307.75</v>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>47.16</v>
-      </c>
-      <c r="C4">
-        <v>59.15</v>
-      </c>
-      <c r="D4">
-        <v>65.02</v>
-      </c>
-      <c r="E4">
-        <v>5272.15</v>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>54.05</v>
-      </c>
-      <c r="C5">
-        <v>61.93</v>
-      </c>
-      <c r="D5">
-        <v>63.58</v>
-      </c>
-      <c r="E5">
-        <v>9789.5</v>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>45.62</v>
-      </c>
-      <c r="C6">
-        <v>58.41</v>
-      </c>
-      <c r="D6">
-        <v>64.90000000000001</v>
-      </c>
-      <c r="E6">
-        <v>1486.75</v>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>48.23</v>
-      </c>
-      <c r="C7">
-        <v>56.84</v>
-      </c>
-      <c r="D7">
-        <v>64.17</v>
-      </c>
-      <c r="E7">
-        <v>691</v>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>51.49</v>
-      </c>
-      <c r="C8">
-        <v>55.32</v>
-      </c>
-      <c r="D8">
-        <v>60.82</v>
-      </c>
-      <c r="E8">
-        <v>2963.35</v>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>41.03</v>
-      </c>
-      <c r="C9">
-        <v>46.38</v>
-      </c>
-      <c r="D9">
-        <v>51.47</v>
-      </c>
-      <c r="E9">
-        <v>6923.9</v>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>49.99</v>
-      </c>
-      <c r="C10">
-        <v>57.04</v>
-      </c>
-      <c r="D10">
-        <v>61.89</v>
-      </c>
-      <c r="E10">
-        <v>3743.05</v>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thursday 03 June 2021 02:59:16 AM IST update
</commit_message>
<xml_diff>
--- a/Record-Data.xlsx
+++ b/Record-Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Daily as on Apr 1, 16:00</t>
   </si>
@@ -257,6 +257,78 @@
   </si>
   <si>
     <t>Closing as on Jun 1, 16:00</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 2, 16:00</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 2, 16:00</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 2, 16:00</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 2, 16:00</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 02, 16:00</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 02, 16:00</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 02, 16:00</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 02, 16:00</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 2, 15:51</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 2, 15:51</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 2, 15:51</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 2, 15:51</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 2, 15:56</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 2, 15:56</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 2, 15:56</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 2, 15:56</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 2, 15:58</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 2, 15:58</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 2, 15:58</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 2, 15:58</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 2, 15:49</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 2, 15:49</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 2, 15:49</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 2, 15:49</t>
   </si>
   <si>
     <t>Name</t>
@@ -731,15 +803,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CD39"/>
+  <dimension ref="A1:DB39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:82">
+    <row r="1" spans="1:106">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -984,10 +1056,82 @@
       <c r="CD1" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="CE1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="2" spans="1:82">
+    <row r="2" spans="1:106">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>45.45</v>
@@ -1196,10 +1340,22 @@
       <c r="CD2">
         <v>2168.9</v>
       </c>
+      <c r="CE2">
+        <v>76.36</v>
+      </c>
+      <c r="CF2">
+        <v>61.93</v>
+      </c>
+      <c r="CG2">
+        <v>65.76000000000001</v>
+      </c>
+      <c r="CH2">
+        <v>2201.25</v>
+      </c>
     </row>
-    <row r="3" spans="1:82">
+    <row r="3" spans="1:106">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>50.2</v>
@@ -1408,10 +1564,22 @@
       <c r="CD3">
         <v>318.1</v>
       </c>
+      <c r="CE3">
+        <v>57.97</v>
+      </c>
+      <c r="CF3">
+        <v>67.72</v>
+      </c>
+      <c r="CG3">
+        <v>65.84</v>
+      </c>
+      <c r="CH3">
+        <v>323</v>
+      </c>
     </row>
-    <row r="4" spans="1:82">
+    <row r="4" spans="1:106">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>47.16</v>
@@ -1620,10 +1788,22 @@
       <c r="CD4">
         <v>5784.8</v>
       </c>
+      <c r="CE4">
+        <v>64.26000000000001</v>
+      </c>
+      <c r="CF4">
+        <v>63.36</v>
+      </c>
+      <c r="CG4">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="CH4">
+        <v>5808.65</v>
+      </c>
     </row>
-    <row r="5" spans="1:82">
+    <row r="5" spans="1:106">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <v>54.05</v>
@@ -1832,10 +2012,22 @@
       <c r="CD5">
         <v>11829.9</v>
       </c>
+      <c r="CE5">
+        <v>67.42</v>
+      </c>
+      <c r="CF5">
+        <v>72.68000000000001</v>
+      </c>
+      <c r="CG5">
+        <v>70.27</v>
+      </c>
+      <c r="CH5">
+        <v>11823.6</v>
+      </c>
     </row>
-    <row r="6" spans="1:82">
+    <row r="6" spans="1:106">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <v>45.62</v>
@@ -2044,10 +2236,22 @@
       <c r="CD6">
         <v>1511.7</v>
       </c>
+      <c r="CE6">
+        <v>57.88</v>
+      </c>
+      <c r="CF6">
+        <v>59.44</v>
+      </c>
+      <c r="CG6">
+        <v>63.38</v>
+      </c>
+      <c r="CH6">
+        <v>1504</v>
+      </c>
     </row>
-    <row r="7" spans="1:82">
+    <row r="7" spans="1:106">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>48.23</v>
@@ -2256,10 +2460,22 @@
       <c r="CD7">
         <v>665.25</v>
       </c>
+      <c r="CE7">
+        <v>52.98</v>
+      </c>
+      <c r="CF7">
+        <v>52.33</v>
+      </c>
+      <c r="CG7">
+        <v>61.72</v>
+      </c>
+      <c r="CH7">
+        <v>675.9</v>
+      </c>
     </row>
-    <row r="8" spans="1:82">
+    <row r="8" spans="1:106">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="B8">
         <v>51.49</v>
@@ -2468,10 +2684,22 @@
       <c r="CD8">
         <v>2964.9</v>
       </c>
+      <c r="CE8">
+        <v>69.81999999999999</v>
+      </c>
+      <c r="CF8">
+        <v>57.86</v>
+      </c>
+      <c r="CG8">
+        <v>60.72</v>
+      </c>
+      <c r="CH8">
+        <v>3014.6</v>
+      </c>
     </row>
-    <row r="9" spans="1:82">
+    <row r="9" spans="1:106">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B9">
         <v>41.03</v>
@@ -2680,10 +2908,22 @@
       <c r="CD9">
         <v>7091.15</v>
       </c>
+      <c r="CE9">
+        <v>68.31</v>
+      </c>
+      <c r="CF9">
+        <v>54.17</v>
+      </c>
+      <c r="CG9">
+        <v>53.59</v>
+      </c>
+      <c r="CH9">
+        <v>7184.7</v>
+      </c>
     </row>
-    <row r="10" spans="1:82">
+    <row r="10" spans="1:106">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B10">
         <v>49.99</v>
@@ -2892,10 +3132,22 @@
       <c r="CD10">
         <v>4238.95</v>
       </c>
+      <c r="CE10">
+        <v>74.12</v>
+      </c>
+      <c r="CF10">
+        <v>71.04000000000001</v>
+      </c>
+      <c r="CG10">
+        <v>68.69</v>
+      </c>
+      <c r="CH10">
+        <v>4295.05</v>
+      </c>
     </row>
-    <row r="11" spans="1:82">
+    <row r="11" spans="1:106">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="B11">
         <v>43.07</v>
@@ -3092,10 +3344,22 @@
       <c r="CD11">
         <v>57.55</v>
       </c>
+      <c r="CE11">
+        <v>63.11</v>
+      </c>
+      <c r="CF11">
+        <v>64.28</v>
+      </c>
+      <c r="CG11">
+        <v>64.13</v>
+      </c>
+      <c r="CH11">
+        <v>60.95</v>
+      </c>
     </row>
-    <row r="12" spans="1:82">
+    <row r="12" spans="1:106">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="B12">
         <v>50.76</v>
@@ -3304,10 +3568,22 @@
       <c r="CD12">
         <v>326</v>
       </c>
+      <c r="CE12">
+        <v>57.74</v>
+      </c>
+      <c r="CF12">
+        <v>62.29</v>
+      </c>
+      <c r="CG12">
+        <v>53.82</v>
+      </c>
+      <c r="CH12">
+        <v>342.3</v>
+      </c>
     </row>
-    <row r="13" spans="1:82">
+    <row r="13" spans="1:106">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B13">
         <v>52.29</v>
@@ -3516,10 +3792,22 @@
       <c r="CD13">
         <v>211.4</v>
       </c>
+      <c r="CE13">
+        <v>56.84</v>
+      </c>
+      <c r="CF13">
+        <v>65.94</v>
+      </c>
+      <c r="CG13">
+        <v>68.97</v>
+      </c>
+      <c r="CH13">
+        <v>223.7</v>
+      </c>
     </row>
-    <row r="14" spans="1:82">
+    <row r="14" spans="1:106">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="B14">
         <v>59.05</v>
@@ -3728,10 +4016,22 @@
       <c r="BZ14">
         <v>2081.95</v>
       </c>
+      <c r="CI14">
+        <v>44.46</v>
+      </c>
+      <c r="CJ14">
+        <v>64.22</v>
+      </c>
+      <c r="CK14">
+        <v>61.99</v>
+      </c>
+      <c r="CL14">
+        <v>2081.6</v>
+      </c>
     </row>
-    <row r="15" spans="1:82">
+    <row r="15" spans="1:106">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="B15">
         <v>41.86</v>
@@ -3940,10 +4240,22 @@
       <c r="CD15">
         <v>532.9</v>
       </c>
+      <c r="CE15">
+        <v>45.52</v>
+      </c>
+      <c r="CF15">
+        <v>49.13</v>
+      </c>
+      <c r="CG15">
+        <v>58.03</v>
+      </c>
+      <c r="CH15">
+        <v>529.5</v>
+      </c>
     </row>
-    <row r="16" spans="1:82">
+    <row r="16" spans="1:106">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B16">
         <v>39.57</v>
@@ -4152,10 +4464,22 @@
       <c r="CD16">
         <v>147.6</v>
       </c>
+      <c r="CE16">
+        <v>60.07</v>
+      </c>
+      <c r="CF16">
+        <v>59.15</v>
+      </c>
+      <c r="CG16">
+        <v>44.67</v>
+      </c>
+      <c r="CH16">
+        <v>149.1</v>
+      </c>
     </row>
-    <row r="17" spans="1:82">
+    <row r="17" spans="1:102">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="B17">
         <v>48.86</v>
@@ -4364,10 +4688,22 @@
       <c r="CD17">
         <v>542.8</v>
       </c>
+      <c r="CE17">
+        <v>72.55</v>
+      </c>
+      <c r="CF17">
+        <v>76.58</v>
+      </c>
+      <c r="CG17">
+        <v>83.81</v>
+      </c>
+      <c r="CH17">
+        <v>543</v>
+      </c>
     </row>
-    <row r="18" spans="1:82">
+    <row r="18" spans="1:102">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="B18">
         <v>42.67</v>
@@ -4576,10 +4912,22 @@
       <c r="CD18">
         <v>221.7</v>
       </c>
+      <c r="CE18">
+        <v>71.59999999999999</v>
+      </c>
+      <c r="CF18">
+        <v>57.84</v>
+      </c>
+      <c r="CG18">
+        <v>42.36</v>
+      </c>
+      <c r="CH18">
+        <v>226.95</v>
+      </c>
     </row>
-    <row r="19" spans="1:82">
+    <row r="19" spans="1:102">
       <c r="A19" s="1" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B19">
         <v>47.21</v>
@@ -4788,10 +5136,22 @@
       <c r="CD19">
         <v>8.5</v>
       </c>
+      <c r="CE19">
+        <v>54.1</v>
+      </c>
+      <c r="CF19">
+        <v>44.61</v>
+      </c>
+      <c r="CG19">
+        <v>39.92</v>
+      </c>
+      <c r="CH19">
+        <v>8.800000000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:82">
+    <row r="20" spans="1:102">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B20">
         <v>48.65</v>
@@ -5000,10 +5360,22 @@
       <c r="CD20">
         <v>1010.05</v>
       </c>
+      <c r="CQ20">
+        <v>63.95</v>
+      </c>
+      <c r="CR20">
+        <v>59.58</v>
+      </c>
+      <c r="CS20">
+        <v>50.84</v>
+      </c>
+      <c r="CT20">
+        <v>1028</v>
+      </c>
     </row>
-    <row r="21" spans="1:82">
+    <row r="21" spans="1:102">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="B21">
         <v>41.16</v>
@@ -5212,10 +5584,22 @@
       <c r="CD21">
         <v>109.9</v>
       </c>
+      <c r="CE21">
+        <v>69.93000000000001</v>
+      </c>
+      <c r="CF21">
+        <v>66.73</v>
+      </c>
+      <c r="CG21">
+        <v>51.38</v>
+      </c>
+      <c r="CH21">
+        <v>110.85</v>
+      </c>
     </row>
-    <row r="22" spans="1:82">
+    <row r="22" spans="1:102">
       <c r="A22" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>45.84</v>
@@ -5412,10 +5796,22 @@
       <c r="CD22">
         <v>1894.6</v>
       </c>
+      <c r="CU22">
+        <v>64.31999999999999</v>
+      </c>
+      <c r="CV22">
+        <v>63.39</v>
+      </c>
+      <c r="CW22">
+        <v>69.45</v>
+      </c>
+      <c r="CX22">
+        <v>1917.95</v>
+      </c>
     </row>
-    <row r="23" spans="1:82">
+    <row r="23" spans="1:102">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B23">
         <v>57.52</v>
@@ -5624,10 +6020,22 @@
       <c r="CD23">
         <v>215.25</v>
       </c>
+      <c r="CE23">
+        <v>48.96</v>
+      </c>
+      <c r="CF23">
+        <v>50.94</v>
+      </c>
+      <c r="CG23">
+        <v>47.18</v>
+      </c>
+      <c r="CH23">
+        <v>209</v>
+      </c>
     </row>
-    <row r="24" spans="1:82">
+    <row r="24" spans="1:102">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="B24">
         <v>50.63</v>
@@ -5836,10 +6244,22 @@
       <c r="CD24">
         <v>1474.65</v>
       </c>
+      <c r="CE24">
+        <v>63.38</v>
+      </c>
+      <c r="CF24">
+        <v>62.63</v>
+      </c>
+      <c r="CG24">
+        <v>60.76</v>
+      </c>
+      <c r="CH24">
+        <v>1471.05</v>
+      </c>
     </row>
-    <row r="25" spans="1:82">
+    <row r="25" spans="1:102">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="B25">
         <v>50.27</v>
@@ -6048,10 +6468,22 @@
       <c r="CD25">
         <v>160</v>
       </c>
+      <c r="CE25">
+        <v>50.32</v>
+      </c>
+      <c r="CF25">
+        <v>45.75</v>
+      </c>
+      <c r="CG25">
+        <v>47.37</v>
+      </c>
+      <c r="CH25">
+        <v>162.85</v>
+      </c>
     </row>
-    <row r="26" spans="1:82">
+    <row r="26" spans="1:102">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B26">
         <v>45.61</v>
@@ -6260,10 +6692,22 @@
       <c r="CD26">
         <v>160.7</v>
       </c>
+      <c r="CE26">
+        <v>61.07</v>
+      </c>
+      <c r="CF26">
+        <v>53.23</v>
+      </c>
+      <c r="CG26">
+        <v>54.57</v>
+      </c>
+      <c r="CH26">
+        <v>163.8</v>
+      </c>
     </row>
-    <row r="27" spans="1:82">
+    <row r="27" spans="1:102">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="B27">
         <v>43.41</v>
@@ -6472,10 +6916,22 @@
       <c r="CD27">
         <v>1308.9</v>
       </c>
+      <c r="CE27">
+        <v>76.68000000000001</v>
+      </c>
+      <c r="CF27">
+        <v>65.44</v>
+      </c>
+      <c r="CG27">
+        <v>67.33</v>
+      </c>
+      <c r="CH27">
+        <v>1414.9</v>
+      </c>
     </row>
-    <row r="28" spans="1:82">
+    <row r="28" spans="1:102">
       <c r="A28" s="1" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B28">
         <v>37.58</v>
@@ -6684,10 +7140,22 @@
       <c r="CD28">
         <v>119.15</v>
       </c>
+      <c r="CE28">
+        <v>63.66</v>
+      </c>
+      <c r="CF28">
+        <v>57.48</v>
+      </c>
+      <c r="CG28">
+        <v>56.57</v>
+      </c>
+      <c r="CH28">
+        <v>121.6</v>
+      </c>
     </row>
-    <row r="29" spans="1:82">
+    <row r="29" spans="1:102">
       <c r="A29" s="1" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B29">
         <v>47.48</v>
@@ -6896,10 +7364,22 @@
       <c r="CD29">
         <v>966.3</v>
       </c>
+      <c r="CE29">
+        <v>58.71</v>
+      </c>
+      <c r="CF29">
+        <v>64.5</v>
+      </c>
+      <c r="CG29">
+        <v>61.68</v>
+      </c>
+      <c r="CH29">
+        <v>984.4</v>
+      </c>
     </row>
-    <row r="30" spans="1:82">
+    <row r="30" spans="1:102">
       <c r="A30" s="1" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="B30">
         <v>49.8</v>
@@ -7108,10 +7588,22 @@
       <c r="CD30">
         <v>432.55</v>
       </c>
+      <c r="CE30">
+        <v>80.81999999999999</v>
+      </c>
+      <c r="CF30">
+        <v>74.68000000000001</v>
+      </c>
+      <c r="CG30">
+        <v>67.58</v>
+      </c>
+      <c r="CH30">
+        <v>437.25</v>
+      </c>
     </row>
-    <row r="31" spans="1:82">
+    <row r="31" spans="1:102">
       <c r="A31" s="1" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="B31">
         <v>56.54</v>
@@ -7308,10 +7800,22 @@
       <c r="CD31">
         <v>104.65</v>
       </c>
+      <c r="CE31">
+        <v>58.7</v>
+      </c>
+      <c r="CF31">
+        <v>67.92</v>
+      </c>
+      <c r="CG31">
+        <v>71.01000000000001</v>
+      </c>
+      <c r="CH31">
+        <v>108.1</v>
+      </c>
     </row>
-    <row r="32" spans="1:82">
+    <row r="32" spans="1:102">
       <c r="A32" s="1" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B32">
         <v>58.02</v>
@@ -7520,10 +8024,22 @@
       <c r="CD32">
         <v>3153</v>
       </c>
+      <c r="CE32">
+        <v>51.33</v>
+      </c>
+      <c r="CF32">
+        <v>56.36</v>
+      </c>
+      <c r="CG32">
+        <v>67.94</v>
+      </c>
+      <c r="CH32">
+        <v>3129.45</v>
+      </c>
     </row>
-    <row r="33" spans="1:82">
+    <row r="33" spans="1:106">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B33">
         <v>64.37</v>
@@ -7720,10 +8236,22 @@
       <c r="CD33">
         <v>706.4</v>
       </c>
+      <c r="CY33">
+        <v>49.11</v>
+      </c>
+      <c r="CZ33">
+        <v>58.83</v>
+      </c>
+      <c r="DA33">
+        <v>60.14</v>
+      </c>
+      <c r="DB33">
+        <v>711.85</v>
+      </c>
     </row>
-    <row r="34" spans="1:82">
+    <row r="34" spans="1:106">
       <c r="A34" s="1" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="B34">
         <v>53.14</v>
@@ -7920,10 +8448,22 @@
       <c r="CD34">
         <v>10.4</v>
       </c>
+      <c r="CM34">
+        <v>62.82</v>
+      </c>
+      <c r="CN34">
+        <v>63.62</v>
+      </c>
+      <c r="CO34">
+        <v>51.11</v>
+      </c>
+      <c r="CP34">
+        <v>10.25</v>
+      </c>
     </row>
-    <row r="35" spans="1:82">
+    <row r="35" spans="1:106">
       <c r="A35" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B35">
         <v>59.65</v>
@@ -8132,10 +8672,22 @@
       <c r="CD35">
         <v>2931</v>
       </c>
+      <c r="CE35">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="CF35">
+        <v>68.26000000000001</v>
+      </c>
+      <c r="CG35">
+        <v>71.91</v>
+      </c>
+      <c r="CH35">
+        <v>2903.7</v>
+      </c>
     </row>
-    <row r="36" spans="1:82">
+    <row r="36" spans="1:106">
       <c r="A36" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="B36">
         <v>60.25</v>
@@ -8344,10 +8896,22 @@
       <c r="BZ36">
         <v>798.2</v>
       </c>
+      <c r="CE36">
+        <v>64.26000000000001</v>
+      </c>
+      <c r="CF36">
+        <v>69.5</v>
+      </c>
+      <c r="CG36">
+        <v>81.2</v>
+      </c>
+      <c r="CH36">
+        <v>811.5</v>
+      </c>
     </row>
-    <row r="37" spans="1:82">
+    <row r="37" spans="1:106">
       <c r="A37" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B37">
         <v>55.37</v>
@@ -8556,10 +9120,22 @@
       <c r="CD37">
         <v>671.05</v>
       </c>
+      <c r="CE37">
+        <v>51.56</v>
+      </c>
+      <c r="CF37">
+        <v>64.20999999999999</v>
+      </c>
+      <c r="CG37">
+        <v>67.11</v>
+      </c>
+      <c r="CH37">
+        <v>677.45</v>
+      </c>
     </row>
-    <row r="38" spans="1:82">
+    <row r="38" spans="1:106">
       <c r="A38" s="1" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B38">
         <v>71.78</v>
@@ -8768,10 +9344,22 @@
       <c r="CD38">
         <v>1100.9</v>
       </c>
+      <c r="CE38">
+        <v>57.88</v>
+      </c>
+      <c r="CF38">
+        <v>77.89</v>
+      </c>
+      <c r="CG38">
+        <v>79.44</v>
+      </c>
+      <c r="CH38">
+        <v>1124.05</v>
+      </c>
     </row>
-    <row r="39" spans="1:82">
+    <row r="39" spans="1:106">
       <c r="A39" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B39">
         <v>67.78</v>
@@ -8979,6 +9567,18 @@
       </c>
       <c r="CD39">
         <v>1760.35</v>
+      </c>
+      <c r="CE39">
+        <v>49.64</v>
+      </c>
+      <c r="CF39">
+        <v>69.34999999999999</v>
+      </c>
+      <c r="CG39">
+        <v>84.31999999999999</v>
+      </c>
+      <c r="CH39">
+        <v>1752.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saturday 05 June 2021 02:25:54 AM IST update
</commit_message>
<xml_diff>
--- a/Record-Data.xlsx
+++ b/Record-Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Daily as on Apr 1, 16:00</t>
   </si>
@@ -329,6 +329,66 @@
   </si>
   <si>
     <t>Closing as on Jun 2, 15:49</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 4, 16:00</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 4, 16:00</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 4, 16:00</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 4, 16:00</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 4, 15:59</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 4, 15:59</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 4, 15:59</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 4, 15:59</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 4, 15:57</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 4, 15:57</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 4, 15:57</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 4, 15:57</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 4, 15:58</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 4, 15:58</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 4, 15:58</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 4, 15:58</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 4, 15:56</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 4, 15:56</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 4, 15:56</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 4, 15:56</t>
   </si>
   <si>
     <t>Name</t>
@@ -803,15 +863,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DB39"/>
+  <dimension ref="A1:DV39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:106">
+    <row r="1" spans="1:126">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1128,10 +1188,70 @@
       <c r="DB1" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="DC1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="2" spans="1:106">
+    <row r="2" spans="1:126">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B2">
         <v>45.45</v>
@@ -1352,10 +1472,22 @@
       <c r="CH2">
         <v>2201.25</v>
       </c>
+      <c r="DC2">
+        <v>72.70999999999999</v>
+      </c>
+      <c r="DD2">
+        <v>61.45</v>
+      </c>
+      <c r="DE2">
+        <v>65.53</v>
+      </c>
+      <c r="DF2">
+        <v>2190.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:106">
+    <row r="3" spans="1:126">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>50.2</v>
@@ -1576,10 +1708,22 @@
       <c r="CH3">
         <v>323</v>
       </c>
+      <c r="DC3">
+        <v>64.93000000000001</v>
+      </c>
+      <c r="DD3">
+        <v>70.2</v>
+      </c>
+      <c r="DE3">
+        <v>66.98</v>
+      </c>
+      <c r="DF3">
+        <v>334.95</v>
+      </c>
     </row>
-    <row r="4" spans="1:106">
+    <row r="4" spans="1:126">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B4">
         <v>47.16</v>
@@ -1800,10 +1944,22 @@
       <c r="CH4">
         <v>5808.65</v>
       </c>
+      <c r="DC4">
+        <v>69.73</v>
+      </c>
+      <c r="DD4">
+        <v>65.52</v>
+      </c>
+      <c r="DE4">
+        <v>69.48999999999999</v>
+      </c>
+      <c r="DF4">
+        <v>5993.45</v>
+      </c>
     </row>
-    <row r="5" spans="1:106">
+    <row r="5" spans="1:126">
       <c r="A5" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B5">
         <v>54.05</v>
@@ -2024,10 +2180,22 @@
       <c r="CH5">
         <v>11823.6</v>
       </c>
+      <c r="DC5">
+        <v>72.66</v>
+      </c>
+      <c r="DD5">
+        <v>74.47</v>
+      </c>
+      <c r="DE5">
+        <v>71.23999999999999</v>
+      </c>
+      <c r="DF5">
+        <v>12155.65</v>
+      </c>
     </row>
-    <row r="6" spans="1:106">
+    <row r="6" spans="1:126">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B6">
         <v>45.62</v>
@@ -2248,10 +2416,22 @@
       <c r="CH6">
         <v>1504</v>
       </c>
+      <c r="DG6">
+        <v>56.02</v>
+      </c>
+      <c r="DH6">
+        <v>59.05</v>
+      </c>
+      <c r="DI6">
+        <v>63.19</v>
+      </c>
+      <c r="DJ6">
+        <v>1500.95</v>
+      </c>
     </row>
-    <row r="7" spans="1:106">
+    <row r="7" spans="1:126">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="B7">
         <v>48.23</v>
@@ -2472,10 +2652,22 @@
       <c r="CH7">
         <v>675.9</v>
       </c>
+      <c r="DC7">
+        <v>56.23</v>
+      </c>
+      <c r="DD7">
+        <v>53.86</v>
+      </c>
+      <c r="DE7">
+        <v>62.16</v>
+      </c>
+      <c r="DF7">
+        <v>680.9</v>
+      </c>
     </row>
-    <row r="8" spans="1:106">
+    <row r="8" spans="1:126">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="B8">
         <v>51.49</v>
@@ -2696,10 +2888,22 @@
       <c r="CH8">
         <v>3014.6</v>
       </c>
+      <c r="DG8">
+        <v>73.62</v>
+      </c>
+      <c r="DH8">
+        <v>59.72</v>
+      </c>
+      <c r="DI8">
+        <v>61.62</v>
+      </c>
+      <c r="DJ8">
+        <v>3067.6</v>
+      </c>
     </row>
-    <row r="9" spans="1:106">
+    <row r="9" spans="1:126">
       <c r="A9" s="1" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B9">
         <v>41.03</v>
@@ -2920,10 +3124,22 @@
       <c r="CH9">
         <v>7184.7</v>
       </c>
+      <c r="DC9">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="DD9">
+        <v>54.69</v>
+      </c>
+      <c r="DE9">
+        <v>53.82</v>
+      </c>
+      <c r="DF9">
+        <v>7214.7</v>
+      </c>
     </row>
-    <row r="10" spans="1:106">
+    <row r="10" spans="1:126">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B10">
         <v>49.99</v>
@@ -3144,10 +3360,22 @@
       <c r="CH10">
         <v>4295.05</v>
       </c>
+      <c r="DC10">
+        <v>68.45</v>
+      </c>
+      <c r="DD10">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="DE10">
+        <v>68.2</v>
+      </c>
+      <c r="DF10">
+        <v>4250.05</v>
+      </c>
     </row>
-    <row r="11" spans="1:106">
+    <row r="11" spans="1:126">
       <c r="A11" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B11">
         <v>43.07</v>
@@ -3356,10 +3584,22 @@
       <c r="CH11">
         <v>60.95</v>
       </c>
+      <c r="DC11">
+        <v>58.42</v>
+      </c>
+      <c r="DD11">
+        <v>63.02</v>
+      </c>
+      <c r="DE11">
+        <v>63.47</v>
+      </c>
+      <c r="DF11">
+        <v>59.8</v>
+      </c>
     </row>
-    <row r="12" spans="1:106">
+    <row r="12" spans="1:126">
       <c r="A12" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B12">
         <v>50.76</v>
@@ -3580,10 +3820,22 @@
       <c r="CH12">
         <v>342.3</v>
       </c>
+      <c r="DC12">
+        <v>69.06999999999999</v>
+      </c>
+      <c r="DD12">
+        <v>68.03</v>
+      </c>
+      <c r="DE12">
+        <v>56.36</v>
+      </c>
+      <c r="DF12">
+        <v>377</v>
+      </c>
     </row>
-    <row r="13" spans="1:106">
+    <row r="13" spans="1:126">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B13">
         <v>52.29</v>
@@ -3804,10 +4056,22 @@
       <c r="CH13">
         <v>223.7</v>
       </c>
+      <c r="DO13">
+        <v>56.83</v>
+      </c>
+      <c r="DP13">
+        <v>66.22</v>
+      </c>
+      <c r="DQ13">
+        <v>69.09</v>
+      </c>
+      <c r="DR13">
+        <v>224.4</v>
+      </c>
     </row>
-    <row r="14" spans="1:106">
+    <row r="14" spans="1:126">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B14">
         <v>59.05</v>
@@ -4028,10 +4292,22 @@
       <c r="CL14">
         <v>2081.6</v>
       </c>
+      <c r="DC14">
+        <v>54.51</v>
+      </c>
+      <c r="DD14">
+        <v>69.48</v>
+      </c>
+      <c r="DE14">
+        <v>64.09</v>
+      </c>
+      <c r="DF14">
+        <v>2248.95</v>
+      </c>
     </row>
-    <row r="15" spans="1:106">
+    <row r="15" spans="1:126">
       <c r="A15" s="1" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="B15">
         <v>41.86</v>
@@ -4252,10 +4528,22 @@
       <c r="CH15">
         <v>529.5</v>
       </c>
+      <c r="DC15">
+        <v>47.71</v>
+      </c>
+      <c r="DD15">
+        <v>49.87</v>
+      </c>
+      <c r="DE15">
+        <v>58.52</v>
+      </c>
+      <c r="DF15">
+        <v>532.7</v>
+      </c>
     </row>
-    <row r="16" spans="1:106">
+    <row r="16" spans="1:126">
       <c r="A16" s="1" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="B16">
         <v>39.57</v>
@@ -4476,10 +4764,22 @@
       <c r="CH16">
         <v>149.1</v>
       </c>
+      <c r="DC16">
+        <v>65.28</v>
+      </c>
+      <c r="DD16">
+        <v>61.5</v>
+      </c>
+      <c r="DE16">
+        <v>45.95</v>
+      </c>
+      <c r="DF16">
+        <v>153.1</v>
+      </c>
     </row>
-    <row r="17" spans="1:102">
+    <row r="17" spans="1:122">
       <c r="A17" s="1" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B17">
         <v>48.86</v>
@@ -4700,10 +5000,22 @@
       <c r="CH17">
         <v>543</v>
       </c>
+      <c r="DO17">
+        <v>69.8</v>
+      </c>
+      <c r="DP17">
+        <v>76.37</v>
+      </c>
+      <c r="DQ17">
+        <v>83.70999999999999</v>
+      </c>
+      <c r="DR17">
+        <v>541.2</v>
+      </c>
     </row>
-    <row r="18" spans="1:102">
+    <row r="18" spans="1:122">
       <c r="A18" s="1" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="B18">
         <v>42.67</v>
@@ -4924,10 +5236,22 @@
       <c r="CH18">
         <v>226.95</v>
       </c>
+      <c r="DC18">
+        <v>83.43000000000001</v>
+      </c>
+      <c r="DD18">
+        <v>64.92</v>
+      </c>
+      <c r="DE18">
+        <v>45.01</v>
+      </c>
+      <c r="DF18">
+        <v>261.35</v>
+      </c>
     </row>
-    <row r="19" spans="1:102">
+    <row r="19" spans="1:122">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B19">
         <v>47.21</v>
@@ -5148,10 +5472,22 @@
       <c r="CH19">
         <v>8.800000000000001</v>
       </c>
+      <c r="DC19">
+        <v>70.05</v>
+      </c>
+      <c r="DD19">
+        <v>51.3</v>
+      </c>
+      <c r="DE19">
+        <v>42.41</v>
+      </c>
+      <c r="DF19">
+        <v>9.75</v>
+      </c>
     </row>
-    <row r="20" spans="1:102">
+    <row r="20" spans="1:122">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B20">
         <v>48.65</v>
@@ -5372,10 +5708,22 @@
       <c r="CT20">
         <v>1028</v>
       </c>
+      <c r="DK20">
+        <v>58.37</v>
+      </c>
+      <c r="DL20">
+        <v>58</v>
+      </c>
+      <c r="DM20">
+        <v>50.24</v>
+      </c>
+      <c r="DN20">
+        <v>1009.3</v>
+      </c>
     </row>
-    <row r="21" spans="1:102">
+    <row r="21" spans="1:122">
       <c r="A21" s="1" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B21">
         <v>41.16</v>
@@ -5596,10 +5944,22 @@
       <c r="CH21">
         <v>110.85</v>
       </c>
+      <c r="DC21">
+        <v>75.03</v>
+      </c>
+      <c r="DD21">
+        <v>69.19</v>
+      </c>
+      <c r="DE21">
+        <v>53.06</v>
+      </c>
+      <c r="DF21">
+        <v>114.6</v>
+      </c>
     </row>
-    <row r="22" spans="1:102">
+    <row r="22" spans="1:122">
       <c r="A22" s="1" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B22">
         <v>45.84</v>
@@ -5808,10 +6168,22 @@
       <c r="CX22">
         <v>1917.95</v>
       </c>
+      <c r="DC22">
+        <v>64.73999999999999</v>
+      </c>
+      <c r="DD22">
+        <v>63.54</v>
+      </c>
+      <c r="DE22">
+        <v>69.51000000000001</v>
+      </c>
+      <c r="DF22">
+        <v>1921.7</v>
+      </c>
     </row>
-    <row r="23" spans="1:102">
+    <row r="23" spans="1:122">
       <c r="A23" s="1" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B23">
         <v>57.52</v>
@@ -6032,10 +6404,22 @@
       <c r="CH23">
         <v>209</v>
       </c>
+      <c r="DC23">
+        <v>48.49</v>
+      </c>
+      <c r="DD23">
+        <v>50.81</v>
+      </c>
+      <c r="DE23">
+        <v>47.11</v>
+      </c>
+      <c r="DF23">
+        <v>208.75</v>
+      </c>
     </row>
-    <row r="24" spans="1:102">
+    <row r="24" spans="1:122">
       <c r="A24" s="1" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B24">
         <v>50.63</v>
@@ -6256,10 +6640,22 @@
       <c r="CH24">
         <v>1471.05</v>
       </c>
+      <c r="DC24">
+        <v>73.45999999999999</v>
+      </c>
+      <c r="DD24">
+        <v>67.23999999999999</v>
+      </c>
+      <c r="DE24">
+        <v>62.94</v>
+      </c>
+      <c r="DF24">
+        <v>1537.55</v>
+      </c>
     </row>
-    <row r="25" spans="1:102">
+    <row r="25" spans="1:122">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="B25">
         <v>50.27</v>
@@ -6480,10 +6876,22 @@
       <c r="CH25">
         <v>162.85</v>
       </c>
+      <c r="DC25">
+        <v>56.24</v>
+      </c>
+      <c r="DD25">
+        <v>48.11</v>
+      </c>
+      <c r="DE25">
+        <v>48.38</v>
+      </c>
+      <c r="DF25">
+        <v>168.15</v>
+      </c>
     </row>
-    <row r="26" spans="1:102">
+    <row r="26" spans="1:122">
       <c r="A26" s="1" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="B26">
         <v>45.61</v>
@@ -6704,10 +7112,22 @@
       <c r="CH26">
         <v>163.8</v>
       </c>
+      <c r="DC26">
+        <v>58.36</v>
+      </c>
+      <c r="DD26">
+        <v>52.41</v>
+      </c>
+      <c r="DE26">
+        <v>54.25</v>
+      </c>
+      <c r="DF26">
+        <v>162.45</v>
+      </c>
     </row>
-    <row r="27" spans="1:102">
+    <row r="27" spans="1:122">
       <c r="A27" s="1" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="B27">
         <v>43.41</v>
@@ -6928,10 +7348,22 @@
       <c r="CH27">
         <v>1414.9</v>
       </c>
+      <c r="DC27">
+        <v>81.72</v>
+      </c>
+      <c r="DD27">
+        <v>69.68000000000001</v>
+      </c>
+      <c r="DE27">
+        <v>69.54000000000001</v>
+      </c>
+      <c r="DF27">
+        <v>1509.35</v>
+      </c>
     </row>
-    <row r="28" spans="1:102">
+    <row r="28" spans="1:122">
       <c r="A28" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B28">
         <v>37.58</v>
@@ -7152,10 +7584,22 @@
       <c r="CH28">
         <v>121.6</v>
       </c>
+      <c r="DC28">
+        <v>63.78</v>
+      </c>
+      <c r="DD28">
+        <v>57.96</v>
+      </c>
+      <c r="DE28">
+        <v>56.78</v>
+      </c>
+      <c r="DF28">
+        <v>122.2</v>
+      </c>
     </row>
-    <row r="29" spans="1:102">
+    <row r="29" spans="1:122">
       <c r="A29" s="1" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B29">
         <v>47.48</v>
@@ -7376,10 +7820,22 @@
       <c r="CH29">
         <v>984.4</v>
       </c>
+      <c r="DC29">
+        <v>60.26</v>
+      </c>
+      <c r="DD29">
+        <v>65.12</v>
+      </c>
+      <c r="DE29">
+        <v>61.95</v>
+      </c>
+      <c r="DF29">
+        <v>989.15</v>
+      </c>
     </row>
-    <row r="30" spans="1:102">
+    <row r="30" spans="1:122">
       <c r="A30" s="1" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B30">
         <v>49.8</v>
@@ -7600,10 +8056,22 @@
       <c r="CH30">
         <v>437.25</v>
       </c>
+      <c r="DC30">
+        <v>75</v>
+      </c>
+      <c r="DD30">
+        <v>74.22</v>
+      </c>
+      <c r="DE30">
+        <v>67.3</v>
+      </c>
+      <c r="DF30">
+        <v>433.6</v>
+      </c>
     </row>
-    <row r="31" spans="1:102">
+    <row r="31" spans="1:122">
       <c r="A31" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B31">
         <v>56.54</v>
@@ -7812,10 +8280,22 @@
       <c r="CH31">
         <v>108.1</v>
       </c>
+      <c r="DC31">
+        <v>58.33</v>
+      </c>
+      <c r="DD31">
+        <v>67.95999999999999</v>
+      </c>
+      <c r="DE31">
+        <v>71.03</v>
+      </c>
+      <c r="DF31">
+        <v>108.15</v>
+      </c>
     </row>
-    <row r="32" spans="1:102">
+    <row r="32" spans="1:122">
       <c r="A32" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B32">
         <v>58.02</v>
@@ -8036,10 +8516,22 @@
       <c r="CH32">
         <v>3129.45</v>
       </c>
+      <c r="DC32">
+        <v>53.44</v>
+      </c>
+      <c r="DD32">
+        <v>57.15</v>
+      </c>
+      <c r="DE32">
+        <v>68.45999999999999</v>
+      </c>
+      <c r="DF32">
+        <v>3143.75</v>
+      </c>
     </row>
-    <row r="33" spans="1:106">
+    <row r="33" spans="1:126">
       <c r="A33" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B33">
         <v>64.37</v>
@@ -8248,10 +8740,22 @@
       <c r="DB33">
         <v>711.85</v>
       </c>
+      <c r="DS33">
+        <v>60.29</v>
+      </c>
+      <c r="DT33">
+        <v>61.83</v>
+      </c>
+      <c r="DU33">
+        <v>61.78</v>
+      </c>
+      <c r="DV33">
+        <v>746.15</v>
+      </c>
     </row>
-    <row r="34" spans="1:106">
+    <row r="34" spans="1:126">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B34">
         <v>53.14</v>
@@ -8460,10 +8964,22 @@
       <c r="CP34">
         <v>10.25</v>
       </c>
+      <c r="DC34">
+        <v>63.11</v>
+      </c>
+      <c r="DD34">
+        <v>65.26000000000001</v>
+      </c>
+      <c r="DE34">
+        <v>51.63</v>
+      </c>
+      <c r="DF34">
+        <v>10.45</v>
+      </c>
     </row>
-    <row r="35" spans="1:106">
+    <row r="35" spans="1:126">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B35">
         <v>59.65</v>
@@ -8684,10 +9200,22 @@
       <c r="CH35">
         <v>2903.7</v>
       </c>
+      <c r="DC35">
+        <v>66.15000000000001</v>
+      </c>
+      <c r="DD35">
+        <v>69.63</v>
+      </c>
+      <c r="DE35">
+        <v>72.66</v>
+      </c>
+      <c r="DF35">
+        <v>2924.9</v>
+      </c>
     </row>
-    <row r="36" spans="1:106">
+    <row r="36" spans="1:126">
       <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="B36">
         <v>60.25</v>
@@ -8908,10 +9436,22 @@
       <c r="CH36">
         <v>811.5</v>
       </c>
+      <c r="DC36">
+        <v>68.51000000000001</v>
+      </c>
+      <c r="DD36">
+        <v>71.02</v>
+      </c>
+      <c r="DE36">
+        <v>81.92</v>
+      </c>
+      <c r="DF36">
+        <v>833.85</v>
+      </c>
     </row>
-    <row r="37" spans="1:106">
+    <row r="37" spans="1:126">
       <c r="A37" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B37">
         <v>55.37</v>
@@ -9132,10 +9672,22 @@
       <c r="CH37">
         <v>677.45</v>
       </c>
+      <c r="DC37">
+        <v>49.86</v>
+      </c>
+      <c r="DD37">
+        <v>63.64</v>
+      </c>
+      <c r="DE37">
+        <v>66.84</v>
+      </c>
+      <c r="DF37">
+        <v>673.95</v>
+      </c>
     </row>
-    <row r="38" spans="1:106">
+    <row r="38" spans="1:126">
       <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="B38">
         <v>71.78</v>
@@ -9356,10 +9908,22 @@
       <c r="CH38">
         <v>1124.05</v>
       </c>
+      <c r="DC38">
+        <v>57.23</v>
+      </c>
+      <c r="DD38">
+        <v>77.76000000000001</v>
+      </c>
+      <c r="DE38">
+        <v>79.15000000000001</v>
+      </c>
+      <c r="DF38">
+        <v>1120.7</v>
+      </c>
     </row>
-    <row r="39" spans="1:106">
+    <row r="39" spans="1:126">
       <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B39">
         <v>67.78</v>
@@ -9579,6 +10143,18 @@
       </c>
       <c r="CH39">
         <v>1752.35</v>
+      </c>
+      <c r="DC39">
+        <v>46.72</v>
+      </c>
+      <c r="DD39">
+        <v>67.81999999999999</v>
+      </c>
+      <c r="DE39">
+        <v>83.04000000000001</v>
+      </c>
+      <c r="DF39">
+        <v>1731.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monday 07 June 2021 11:43:59 PM IST update
</commit_message>
<xml_diff>
--- a/Record-Data.xlsx
+++ b/Record-Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Daily as on Apr 1, 16:00</t>
   </si>
@@ -389,6 +389,18 @@
   </si>
   <si>
     <t>Closing as on Jun 4, 15:56</t>
+  </si>
+  <si>
+    <t>Daily as on Jun 7, 16:00</t>
+  </si>
+  <si>
+    <t>Weekly as on Jun 7, 16:00</t>
+  </si>
+  <si>
+    <t>Monthly as on Jun 7, 16:00</t>
+  </si>
+  <si>
+    <t>Closing as on Jun 7, 16:00</t>
   </si>
   <si>
     <t>Name</t>
@@ -863,15 +875,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DV39"/>
+  <dimension ref="A1:DZ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:126">
+    <row r="1" spans="1:130">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1248,10 +1260,22 @@
       <c r="DV1" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="DW1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:126">
+    <row r="2" spans="1:130">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>45.45</v>
@@ -1484,10 +1508,22 @@
       <c r="DF2">
         <v>2190.5</v>
       </c>
+      <c r="DW2">
+        <v>75.48999999999999</v>
+      </c>
+      <c r="DX2">
+        <v>63.17</v>
+      </c>
+      <c r="DY2">
+        <v>66.31</v>
+      </c>
+      <c r="DZ2">
+        <v>2227.4</v>
+      </c>
     </row>
-    <row r="3" spans="1:126">
+    <row r="3" spans="1:130">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3">
         <v>50.2</v>
@@ -1720,10 +1756,22 @@
       <c r="DF3">
         <v>334.95</v>
       </c>
+      <c r="DW3">
+        <v>69.77</v>
+      </c>
+      <c r="DX3">
+        <v>72.23</v>
+      </c>
+      <c r="DY3">
+        <v>67.92</v>
+      </c>
+      <c r="DZ3">
+        <v>345.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:126">
+    <row r="4" spans="1:130">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>47.16</v>
@@ -1956,10 +2004,22 @@
       <c r="DF4">
         <v>5993.45</v>
       </c>
+      <c r="DW4">
+        <v>56.05</v>
+      </c>
+      <c r="DX4">
+        <v>60.09</v>
+      </c>
+      <c r="DY4">
+        <v>67.91</v>
+      </c>
+      <c r="DZ4">
+        <v>5729.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:126">
+    <row r="5" spans="1:130">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B5">
         <v>54.05</v>
@@ -2192,10 +2252,22 @@
       <c r="DF5">
         <v>12155.65</v>
       </c>
+      <c r="DW5">
+        <v>61.97</v>
+      </c>
+      <c r="DX5">
+        <v>69.64</v>
+      </c>
+      <c r="DY5">
+        <v>70.29000000000001</v>
+      </c>
+      <c r="DZ5">
+        <v>11828.55</v>
+      </c>
     </row>
-    <row r="6" spans="1:126">
+    <row r="6" spans="1:130">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>45.62</v>
@@ -2428,10 +2500,22 @@
       <c r="DJ6">
         <v>1500.95</v>
       </c>
+      <c r="DW6">
+        <v>55.77</v>
+      </c>
+      <c r="DX6">
+        <v>58.89</v>
+      </c>
+      <c r="DY6">
+        <v>63.12</v>
+      </c>
+      <c r="DZ6">
+        <v>1499.85</v>
+      </c>
     </row>
-    <row r="7" spans="1:126">
+    <row r="7" spans="1:130">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B7">
         <v>48.23</v>
@@ -2664,10 +2748,22 @@
       <c r="DF7">
         <v>680.9</v>
       </c>
+      <c r="DW7">
+        <v>55.54</v>
+      </c>
+      <c r="DX7">
+        <v>53.56</v>
+      </c>
+      <c r="DY7">
+        <v>62.09</v>
+      </c>
+      <c r="DZ7">
+        <v>680.1</v>
+      </c>
     </row>
-    <row r="8" spans="1:126">
+    <row r="8" spans="1:130">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B8">
         <v>51.49</v>
@@ -2900,10 +2996,22 @@
       <c r="DJ8">
         <v>3067.6</v>
       </c>
+      <c r="DW8">
+        <v>67.31</v>
+      </c>
+      <c r="DX8">
+        <v>57.9</v>
+      </c>
+      <c r="DY8">
+        <v>61.03</v>
+      </c>
+      <c r="DZ8">
+        <v>3032.7</v>
+      </c>
     </row>
-    <row r="9" spans="1:126">
+    <row r="9" spans="1:130">
       <c r="A9" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>41.03</v>
@@ -3136,10 +3244,22 @@
       <c r="DF9">
         <v>7214.7</v>
       </c>
+      <c r="DW9">
+        <v>71.65000000000001</v>
+      </c>
+      <c r="DX9">
+        <v>55.77</v>
+      </c>
+      <c r="DY9">
+        <v>54.29</v>
+      </c>
+      <c r="DZ9">
+        <v>7275.65</v>
+      </c>
     </row>
-    <row r="10" spans="1:126">
+    <row r="10" spans="1:130">
       <c r="A10" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B10">
         <v>49.99</v>
@@ -3372,10 +3492,22 @@
       <c r="DF10">
         <v>4250.05</v>
       </c>
+      <c r="DW10">
+        <v>68.41</v>
+      </c>
+      <c r="DX10">
+        <v>70.08</v>
+      </c>
+      <c r="DY10">
+        <v>68.19</v>
+      </c>
+      <c r="DZ10">
+        <v>4249.75</v>
+      </c>
     </row>
-    <row r="11" spans="1:126">
+    <row r="11" spans="1:130">
       <c r="A11" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B11">
         <v>43.07</v>
@@ -3596,10 +3728,22 @@
       <c r="DF11">
         <v>59.8</v>
       </c>
+      <c r="DW11">
+        <v>60.12</v>
+      </c>
+      <c r="DX11">
+        <v>63.74</v>
+      </c>
+      <c r="DY11">
+        <v>63.82</v>
+      </c>
+      <c r="DZ11">
+        <v>60.4</v>
+      </c>
     </row>
-    <row r="12" spans="1:126">
+    <row r="12" spans="1:130">
       <c r="A12" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B12">
         <v>50.76</v>
@@ -3832,10 +3976,22 @@
       <c r="DF12">
         <v>377</v>
       </c>
+      <c r="DW12">
+        <v>76.65000000000001</v>
+      </c>
+      <c r="DX12">
+        <v>72.87</v>
+      </c>
+      <c r="DY12">
+        <v>58.82</v>
+      </c>
+      <c r="DZ12">
+        <v>414.7</v>
+      </c>
     </row>
-    <row r="13" spans="1:126">
+    <row r="13" spans="1:130">
       <c r="A13" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B13">
         <v>52.29</v>
@@ -4068,10 +4224,22 @@
       <c r="DR13">
         <v>224.4</v>
       </c>
+      <c r="DW13">
+        <v>67.09999999999999</v>
+      </c>
+      <c r="DX13">
+        <v>71.63</v>
+      </c>
+      <c r="DY13">
+        <v>71.81</v>
+      </c>
+      <c r="DZ13">
+        <v>242.5</v>
+      </c>
     </row>
-    <row r="14" spans="1:126">
+    <row r="14" spans="1:130">
       <c r="A14" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B14">
         <v>59.05</v>
@@ -4304,10 +4472,22 @@
       <c r="DF14">
         <v>2248.95</v>
       </c>
+      <c r="DW14">
+        <v>60.41</v>
+      </c>
+      <c r="DX14">
+        <v>71.73999999999999</v>
+      </c>
+      <c r="DY14">
+        <v>65.41</v>
+      </c>
+      <c r="DZ14">
+        <v>2369.8</v>
+      </c>
     </row>
-    <row r="15" spans="1:126">
+    <row r="15" spans="1:130">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B15">
         <v>41.86</v>
@@ -4540,10 +4720,22 @@
       <c r="DF15">
         <v>532.7</v>
       </c>
+      <c r="DW15">
+        <v>50.38</v>
+      </c>
+      <c r="DX15">
+        <v>50.76</v>
+      </c>
+      <c r="DY15">
+        <v>59.04</v>
+      </c>
+      <c r="DZ15">
+        <v>536.45</v>
+      </c>
     </row>
-    <row r="16" spans="1:126">
+    <row r="16" spans="1:130">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B16">
         <v>39.57</v>
@@ -4776,10 +4968,22 @@
       <c r="DF16">
         <v>153.1</v>
       </c>
+      <c r="DW16">
+        <v>68.76000000000001</v>
+      </c>
+      <c r="DX16">
+        <v>63.3</v>
+      </c>
+      <c r="DY16">
+        <v>46.92</v>
+      </c>
+      <c r="DZ16">
+        <v>156.25</v>
+      </c>
     </row>
-    <row r="17" spans="1:122">
+    <row r="17" spans="1:130">
       <c r="A17" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B17">
         <v>48.86</v>
@@ -5012,10 +5216,22 @@
       <c r="DR17">
         <v>541.2</v>
       </c>
+      <c r="DW17">
+        <v>72.56</v>
+      </c>
+      <c r="DX17">
+        <v>77.23</v>
+      </c>
+      <c r="DY17">
+        <v>84.06999999999999</v>
+      </c>
+      <c r="DZ17">
+        <v>548.25</v>
+      </c>
     </row>
-    <row r="18" spans="1:122">
+    <row r="18" spans="1:130">
       <c r="A18" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B18">
         <v>42.67</v>
@@ -5248,10 +5464,22 @@
       <c r="DF18">
         <v>261.35</v>
       </c>
+      <c r="DW18">
+        <v>70.86</v>
+      </c>
+      <c r="DX18">
+        <v>60.6</v>
+      </c>
+      <c r="DY18">
+        <v>44</v>
+      </c>
+      <c r="DZ18">
+        <v>247.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:122">
+    <row r="19" spans="1:130">
       <c r="A19" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B19">
         <v>47.21</v>
@@ -5484,10 +5712,22 @@
       <c r="DF19">
         <v>9.75</v>
       </c>
+      <c r="DW19">
+        <v>73.81</v>
+      </c>
+      <c r="DX19">
+        <v>53.53</v>
+      </c>
+      <c r="DY19">
+        <v>43.28</v>
+      </c>
+      <c r="DZ19">
+        <v>10.1</v>
+      </c>
     </row>
-    <row r="20" spans="1:122">
+    <row r="20" spans="1:130">
       <c r="A20" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B20">
         <v>48.65</v>
@@ -5720,10 +5960,22 @@
       <c r="DN20">
         <v>1009.3</v>
       </c>
+      <c r="DW20">
+        <v>61.46</v>
+      </c>
+      <c r="DX20">
+        <v>59.16</v>
+      </c>
+      <c r="DY20">
+        <v>50.76</v>
+      </c>
+      <c r="DZ20">
+        <v>1025.2</v>
+      </c>
     </row>
-    <row r="21" spans="1:122">
+    <row r="21" spans="1:130">
       <c r="A21" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B21">
         <v>41.16</v>
@@ -5956,10 +6208,22 @@
       <c r="DF21">
         <v>114.6</v>
       </c>
+      <c r="DW21">
+        <v>75.15000000000001</v>
+      </c>
+      <c r="DX21">
+        <v>69.26000000000001</v>
+      </c>
+      <c r="DY21">
+        <v>53.1</v>
+      </c>
+      <c r="DZ21">
+        <v>114.7</v>
+      </c>
     </row>
-    <row r="22" spans="1:122">
+    <row r="22" spans="1:130">
       <c r="A22" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B22">
         <v>45.84</v>
@@ -6180,10 +6444,22 @@
       <c r="DF22">
         <v>1921.7</v>
       </c>
+      <c r="DW22">
+        <v>78.54000000000001</v>
+      </c>
+      <c r="DX22">
+        <v>69.56999999999999</v>
+      </c>
+      <c r="DY22">
+        <v>72.04000000000001</v>
+      </c>
+      <c r="DZ22">
+        <v>2094.8</v>
+      </c>
     </row>
-    <row r="23" spans="1:122">
+    <row r="23" spans="1:130">
       <c r="A23" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B23">
         <v>57.52</v>
@@ -6416,10 +6692,22 @@
       <c r="DF23">
         <v>208.75</v>
       </c>
+      <c r="DW23">
+        <v>53.6</v>
+      </c>
+      <c r="DX23">
+        <v>52.26</v>
+      </c>
+      <c r="DY23">
+        <v>47.88</v>
+      </c>
+      <c r="DZ23">
+        <v>211.45</v>
+      </c>
     </row>
-    <row r="24" spans="1:122">
+    <row r="24" spans="1:130">
       <c r="A24" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B24">
         <v>50.63</v>
@@ -6652,10 +6940,22 @@
       <c r="DF24">
         <v>1537.55</v>
       </c>
+      <c r="DW24">
+        <v>75.73999999999999</v>
+      </c>
+      <c r="DX24">
+        <v>68.43000000000001</v>
+      </c>
+      <c r="DY24">
+        <v>63.55</v>
+      </c>
+      <c r="DZ24">
+        <v>1557.8</v>
+      </c>
     </row>
-    <row r="25" spans="1:122">
+    <row r="25" spans="1:130">
       <c r="A25" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B25">
         <v>50.27</v>
@@ -6888,10 +7188,22 @@
       <c r="DF25">
         <v>168.15</v>
       </c>
+      <c r="DW25">
+        <v>58.79</v>
+      </c>
+      <c r="DX25">
+        <v>49.25</v>
+      </c>
+      <c r="DY25">
+        <v>48.85</v>
+      </c>
+      <c r="DZ25">
+        <v>170.7</v>
+      </c>
     </row>
-    <row r="26" spans="1:122">
+    <row r="26" spans="1:130">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B26">
         <v>45.61</v>
@@ -7124,10 +7436,22 @@
       <c r="DF26">
         <v>162.45</v>
       </c>
+      <c r="DW26">
+        <v>62.07</v>
+      </c>
+      <c r="DX26">
+        <v>54.3</v>
+      </c>
+      <c r="DY26">
+        <v>54.93</v>
+      </c>
+      <c r="DZ26">
+        <v>165.4</v>
+      </c>
     </row>
-    <row r="27" spans="1:122">
+    <row r="27" spans="1:130">
       <c r="A27" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B27">
         <v>43.41</v>
@@ -7360,10 +7684,22 @@
       <c r="DF27">
         <v>1509.35</v>
       </c>
+      <c r="DW27">
+        <v>81.91</v>
+      </c>
+      <c r="DX27">
+        <v>69.84</v>
+      </c>
+      <c r="DY27">
+        <v>69.62</v>
+      </c>
+      <c r="DZ27">
+        <v>1513.15</v>
+      </c>
     </row>
-    <row r="28" spans="1:122">
+    <row r="28" spans="1:130">
       <c r="A28" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B28">
         <v>37.58</v>
@@ -7596,10 +7932,22 @@
       <c r="DF28">
         <v>122.2</v>
       </c>
+      <c r="DW28">
+        <v>69.53</v>
+      </c>
+      <c r="DX28">
+        <v>60.75</v>
+      </c>
+      <c r="DY28">
+        <v>58</v>
+      </c>
+      <c r="DZ28">
+        <v>125.75</v>
+      </c>
     </row>
-    <row r="29" spans="1:122">
+    <row r="29" spans="1:130">
       <c r="A29" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B29">
         <v>47.48</v>
@@ -7832,10 +8180,22 @@
       <c r="DF29">
         <v>989.15</v>
       </c>
+      <c r="DW29">
+        <v>59.92</v>
+      </c>
+      <c r="DX29">
+        <v>64.95999999999999</v>
+      </c>
+      <c r="DY29">
+        <v>61.91</v>
+      </c>
+      <c r="DZ29">
+        <v>988.5</v>
+      </c>
     </row>
-    <row r="30" spans="1:122">
+    <row r="30" spans="1:130">
       <c r="A30" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B30">
         <v>49.8</v>
@@ -8068,10 +8428,22 @@
       <c r="DF30">
         <v>433.6</v>
       </c>
+      <c r="DW30">
+        <v>73.61</v>
+      </c>
+      <c r="DX30">
+        <v>73.68000000000001</v>
+      </c>
+      <c r="DY30">
+        <v>67.2</v>
+      </c>
+      <c r="DZ30">
+        <v>432.25</v>
+      </c>
     </row>
-    <row r="31" spans="1:122">
+    <row r="31" spans="1:130">
       <c r="A31" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B31">
         <v>56.54</v>
@@ -8292,10 +8664,22 @@
       <c r="DF31">
         <v>108.15</v>
       </c>
+      <c r="DW31">
+        <v>66.68000000000001</v>
+      </c>
+      <c r="DX31">
+        <v>71.31999999999999</v>
+      </c>
+      <c r="DY31">
+        <v>72.64</v>
+      </c>
+      <c r="DZ31">
+        <v>113.35</v>
+      </c>
     </row>
-    <row r="32" spans="1:122">
+    <row r="32" spans="1:130">
       <c r="A32" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B32">
         <v>58.02</v>
@@ -8528,10 +8912,22 @@
       <c r="DF32">
         <v>3143.75</v>
       </c>
+      <c r="DW32">
+        <v>59.03</v>
+      </c>
+      <c r="DX32">
+        <v>58.85</v>
+      </c>
+      <c r="DY32">
+        <v>69.43000000000001</v>
+      </c>
+      <c r="DZ32">
+        <v>3183.2</v>
+      </c>
     </row>
-    <row r="33" spans="1:126">
+    <row r="33" spans="1:130">
       <c r="A33" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B33">
         <v>64.37</v>
@@ -8752,10 +9148,22 @@
       <c r="DV33">
         <v>746.15</v>
       </c>
+      <c r="DW33">
+        <v>60.86</v>
+      </c>
+      <c r="DX33">
+        <v>62.01</v>
+      </c>
+      <c r="DY33">
+        <v>61.87</v>
+      </c>
+      <c r="DZ33">
+        <v>748.2</v>
+      </c>
     </row>
-    <row r="34" spans="1:126">
+    <row r="34" spans="1:130">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B34">
         <v>53.14</v>
@@ -8976,10 +9384,22 @@
       <c r="DF34">
         <v>10.45</v>
       </c>
+      <c r="DW34">
+        <v>67.22</v>
+      </c>
+      <c r="DX34">
+        <v>67.52</v>
+      </c>
+      <c r="DY34">
+        <v>52.97</v>
+      </c>
+      <c r="DZ34">
+        <v>10.95</v>
+      </c>
     </row>
-    <row r="35" spans="1:126">
+    <row r="35" spans="1:130">
       <c r="A35" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B35">
         <v>59.65</v>
@@ -9212,10 +9632,22 @@
       <c r="DF35">
         <v>2924.9</v>
       </c>
+      <c r="DW35">
+        <v>66.81</v>
+      </c>
+      <c r="DX35">
+        <v>69.88</v>
+      </c>
+      <c r="DY35">
+        <v>72.95999999999999</v>
+      </c>
+      <c r="DZ35">
+        <v>2933.1</v>
+      </c>
     </row>
-    <row r="36" spans="1:126">
+    <row r="36" spans="1:130">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B36">
         <v>60.25</v>
@@ -9448,10 +9880,22 @@
       <c r="DF36">
         <v>833.85</v>
       </c>
+      <c r="DW36">
+        <v>75.17</v>
+      </c>
+      <c r="DX36">
+        <v>73.83</v>
+      </c>
+      <c r="DY36">
+        <v>83.22</v>
+      </c>
+      <c r="DZ36">
+        <v>878.6</v>
+      </c>
     </row>
-    <row r="37" spans="1:126">
+    <row r="37" spans="1:130">
       <c r="A37" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B37">
         <v>55.37</v>
@@ -9684,10 +10128,22 @@
       <c r="DF37">
         <v>673.95</v>
       </c>
+      <c r="DW37">
+        <v>50.59</v>
+      </c>
+      <c r="DX37">
+        <v>63.89</v>
+      </c>
+      <c r="DY37">
+        <v>66.95</v>
+      </c>
+      <c r="DZ37">
+        <v>675.35</v>
+      </c>
     </row>
-    <row r="38" spans="1:126">
+    <row r="38" spans="1:130">
       <c r="A38" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B38">
         <v>71.78</v>
@@ -9920,10 +10376,22 @@
       <c r="DF38">
         <v>1120.7</v>
       </c>
+      <c r="DW38">
+        <v>58.48</v>
+      </c>
+      <c r="DX38">
+        <v>78.09999999999999</v>
+      </c>
+      <c r="DY38">
+        <v>79.64</v>
+      </c>
+      <c r="DZ38">
+        <v>1128.7</v>
+      </c>
     </row>
-    <row r="39" spans="1:126">
+    <row r="39" spans="1:130">
       <c r="A39" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B39">
         <v>67.78</v>
@@ -10155,6 +10623,18 @@
       </c>
       <c r="DF39">
         <v>1731.65</v>
+      </c>
+      <c r="DW39">
+        <v>50.3</v>
+      </c>
+      <c r="DX39">
+        <v>68.63</v>
+      </c>
+      <c r="DY39">
+        <v>84.43000000000001</v>
+      </c>
+      <c r="DZ39">
+        <v>1754.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>